<commit_message>
Added otp password test
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/w.xlsx
+++ b/src/test/resources/testData/w.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="9480"/>
+    <workbookView windowWidth="24000" windowHeight="9480" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Web Inputs" sheetId="1" r:id="rId1"/>
+    <sheet name="Login Page" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateCount="100" iterateDelta="0.001"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>run</t>
   </si>
@@ -49,6 +49,18 @@
     <t>text input</t>
   </si>
   <si>
+    <t>Web inputs</t>
+  </si>
+  <si>
+    <t>15/4/2024</t>
+  </si>
+  <si>
+    <t>pass1</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
     <t>su user name</t>
   </si>
   <si>
@@ -64,25 +76,13 @@
     <t>re con pass</t>
   </si>
   <si>
-    <t>Web inputs</t>
-  </si>
-  <si>
-    <t>15/4/2024</t>
-  </si>
-  <si>
-    <t>pass1</t>
-  </si>
-  <si>
-    <t>text1</t>
-  </si>
-  <si>
     <t>Test Login Page</t>
   </si>
   <si>
     <t>test</t>
   </si>
   <si>
-    <t>yfvvsfc</t>
+    <t>tr1111111</t>
   </si>
 </sst>
 </file>
@@ -1263,21 +1263,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G$1:K$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="2" width="11.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="9" max="9" width="12.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" spans="1:11">
+    <row r="1" ht="15" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1295,21 +1293,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1317,43 +1300,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3"/>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="2:2">
@@ -1362,7 +1321,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Web inputs" tooltip="https://practice.expandtesting.com/inputs"/>
-    <hyperlink ref="B3" r:id="rId2" display="Test Login Page" tooltip="https://practice.expandtesting.com/login"/>
   </hyperlinks>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="256" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="600" verticalDpi="600"/>
@@ -1373,14 +1331,73 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="A1:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="6.42857142857143" customWidth="1"/>
+    <col min="2" max="2" width="15.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="13.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="8.14285714285714" customWidth="1"/>
+    <col min="5" max="5" width="12.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="7.71428571428571" customWidth="1"/>
+    <col min="7" max="7" width="11.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="Test Login Page" tooltip="https://practice.expandtesting.com/login"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" errors="NA" horizontalDpi="600" verticalDpi="600"/>
   <headerFooter alignWithMargins="0" scaleWithDoc="0"/>

</xml_diff>

<commit_message>
Added method to start new tab
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/w.xlsx
+++ b/src/test/resources/testData/w.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="9480" activeTab="1"/>
+    <workbookView windowWidth="24000" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="Web Inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Login Page" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="100" iterateDelta="0.001"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1265,8 +1265,8 @@
   <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G$1:K$1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="5"/>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1333,7 +1333,7 @@
   <sheetPr/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Divided the login and register tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/w.xlsx
+++ b/src/test/resources/testData/w.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="9480"/>
+    <workbookView windowWidth="24000" windowHeight="8760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Web Inputs" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>run</t>
   </si>
@@ -61,28 +61,25 @@
     <t>text1</t>
   </si>
   <si>
-    <t>su user name</t>
-  </si>
-  <si>
-    <t>su pass</t>
-  </si>
-  <si>
-    <t>re user name</t>
-  </si>
-  <si>
-    <t>re pass</t>
-  </si>
-  <si>
-    <t>re con pass</t>
-  </si>
-  <si>
-    <t>Test Login Page</t>
+    <t>user name</t>
+  </si>
+  <si>
+    <t>Assertion</t>
+  </si>
+  <si>
+    <t>Successful  Login Page</t>
   </si>
   <si>
     <t>test</t>
   </si>
   <si>
-    <t>tr1111111</t>
+    <t>Failed login</t>
+  </si>
+  <si>
+    <t>tes</t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
 </sst>
 </file>
@@ -733,7 +730,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1265,7 +1262,7 @@
   <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1331,24 +1328,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="6.42857142857143" customWidth="1"/>
     <col min="2" max="2" width="15.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="13.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="8.14285714285714" customWidth="1"/>
-    <col min="5" max="5" width="12.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="7.71428571428571" customWidth="1"/>
-    <col min="7" max="7" width="11.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="14.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1359,44 +1354,49 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:5">
       <c r="A2" t="b">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Test Login Page" tooltip="https://practice.expandtesting.com/login"/>
+    <hyperlink ref="B2" r:id="rId1" display="Successful  Login Page" tooltip="https://practice.expandtesting.com/login"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" errors="NA" horizontalDpi="600" verticalDpi="600"/>

</xml_diff>